<commit_message>
updated eruption averages with vent locations shifted after looking carefully at saemundsson maps
</commit_message>
<xml_diff>
--- a/RVB_min_by_erupt.xlsx
+++ b/RVB_min_by_erupt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/jcm1004_cam_ac_uk/Documents/gmt_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B87280A1-7002-9142-A0D5-B2309FDC980B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{69B918C6-9E72-2B49-B76F-6F8EA25AAE6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13880" yWindow="500" windowWidth="18040" windowHeight="16500"/>
+    <workbookView xWindow="13880" yWindow="500" windowWidth="18040" windowHeight="16480"/>
   </bookViews>
   <sheets>
     <sheet name="RVB_min" sheetId="1" r:id="rId1"/>
@@ -1725,8 +1725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD83" workbookViewId="0">
-      <selection activeCell="AI107" sqref="AI107"/>
+    <sheetView tabSelected="1" topLeftCell="AB93" workbookViewId="0">
+      <selection activeCell="AI90" sqref="AI90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>